<commit_message>
big stimulus update and add definition of prompting trials to generare_trials_localisers
- fix sampling rate of sounds
- make backgrounds more uniform for image stimuli
</commit_message>
<xml_diff>
--- a/sequences/localiser_trials_prc.xlsx
+++ b/sequences/localiser_trials_prc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sync_folder\Study 1 - MEG replay\Experiment\learning-replay-MEG-task\sequences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sync_folder\TSRlearn-task\sequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -143,9 +143,6 @@
     <t>belt</t>
   </si>
   <si>
-    <t xml:space="preserve">bicycle </t>
-  </si>
-  <si>
     <t>left</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>nonmatch_pres_side</t>
+  </si>
+  <si>
+    <t>bicycle</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -542,13 +542,13 @@
         <v>0.89</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -611,13 +611,13 @@
         <v>1.04</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -657,13 +657,13 @@
         <v>0.79</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -703,13 +703,13 @@
         <v>1.23</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -743,7 +743,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1">
         <v>1.25</v>
@@ -755,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>